<commit_message>
adjust form builder (otw on edit, minus validate) filter and table (otw)
</commit_message>
<xml_diff>
--- a/public/assets/ProductImport.xlsx
+++ b/public/assets/ProductImport.xlsx
@@ -4,10 +4,10 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19890" windowHeight="7560"/>
+    <workbookView windowWidth="20130" windowHeight="7560"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Product" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
@@ -110,22 +110,14 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -138,7 +130,85 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -152,107 +222,37 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -267,19 +267,115 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -291,7 +387,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -303,151 +435,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -485,11 +485,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -521,21 +527,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
@@ -558,151 +549,160 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="32" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1047,7 +1047,7 @@
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4285714285714" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="3" outlineLevelCol="7"/>

</xml_diff>